<commit_message>
Comitting the working files for data ingestion
Included
- Apache Beam beginner notebook
- Data ingestion using CSV, TFRecords, sample code chunks on connecting to remote databases like S3.
- Data splitting using TFX
</commit_message>
<xml_diff>
--- a/Concepts.xlsx
+++ b/Concepts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Concepts</t>
   </si>
@@ -69,13 +69,28 @@
   </si>
   <si>
     <t>Data Privacy in ML</t>
+  </si>
+  <si>
+    <t>Sub topics</t>
+  </si>
+  <si>
+    <t>TFX for data ingestion from files/services</t>
+  </si>
+  <si>
+    <t>train-test splits</t>
+  </si>
+  <si>
+    <t>combine multiple data exports into one all-encompassing dataset</t>
+  </si>
+  <si>
+    <t>strategies to ingest different forms of data (structured, text, and images)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +105,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -106,7 +127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -129,15 +150,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,109 +487,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.08984375" customWidth="1"/>
-    <col min="2" max="2" width="87.453125" customWidth="1"/>
+    <col min="1" max="2" width="52.08984375" customWidth="1"/>
+    <col min="3" max="3" width="87.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="5"/>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="6"/>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:A7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>